<commit_message>
All of the 150 rows of sensor data.
</commit_message>
<xml_diff>
--- a/sensor_readings_first50.xlsx
+++ b/sensor_readings_first50.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -466,10 +470,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:00:15</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>45978.37517361111</v>
       </c>
       <c r="B2" t="n">
         <v>27</v>
@@ -486,10 +488,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:00:20</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>45978.37523148148</v>
       </c>
       <c r="B3" t="n">
         <v>30.2</v>
@@ -502,10 +502,8 @@
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:00:35</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>45978.37540509259</v>
       </c>
       <c r="B4" t="n">
         <v>34.8</v>
@@ -522,10 +520,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:00:50</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>45978.3755787037</v>
       </c>
       <c r="B5" t="n">
         <v>32.1</v>
@@ -538,10 +534,8 @@
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:01:00</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>45978.37569444445</v>
       </c>
       <c r="B6" t="n">
         <v>30.4</v>
@@ -558,10 +552,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:01:40</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>45978.37615740741</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
@@ -574,10 +566,8 @@
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:01:45</t>
-        </is>
+      <c r="A8" s="2" t="n">
+        <v>45978.37621527778</v>
       </c>
       <c r="B8" t="n">
         <v>26.6</v>
@@ -592,10 +582,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:01:55</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>45978.37633101852</v>
       </c>
       <c r="B9" t="n">
         <v>40.6</v>
@@ -614,10 +602,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:02:10</t>
-        </is>
+      <c r="A10" s="2" t="n">
+        <v>45978.37650462963</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
@@ -632,10 +618,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:02:20</t>
-        </is>
+      <c r="A11" s="2" t="n">
+        <v>45978.37662037037</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
@@ -648,10 +632,8 @@
       <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:02:50</t>
-        </is>
+      <c r="A12" s="2" t="n">
+        <v>45978.37696759259</v>
       </c>
       <c r="B12" t="n">
         <v>39</v>
@@ -668,10 +650,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:03:10</t>
-        </is>
+      <c r="A13" s="2" t="n">
+        <v>45978.37719907407</v>
       </c>
       <c r="B13" t="n">
         <v>37.6</v>
@@ -682,10 +662,8 @@
       <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:03:25</t>
-        </is>
+      <c r="A14" s="2" t="n">
+        <v>45978.37737268519</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
@@ -696,10 +674,8 @@
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:03:40</t>
-        </is>
+      <c r="A15" s="2" t="n">
+        <v>45978.37754629629</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
@@ -714,10 +690,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:03:55</t>
-        </is>
+      <c r="A16" s="2" t="n">
+        <v>45978.37771990741</v>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
@@ -728,10 +702,8 @@
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:04:10</t>
-        </is>
+      <c r="A17" s="2" t="n">
+        <v>45978.37789351852</v>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
@@ -744,10 +716,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:04:25</t>
-        </is>
+      <c r="A18" s="2" t="n">
+        <v>45978.37806712963</v>
       </c>
       <c r="B18" t="n">
         <v>38</v>
@@ -762,10 +732,8 @@
       <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:04:30</t>
-        </is>
+      <c r="A19" s="2" t="n">
+        <v>45978.378125</v>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
@@ -776,10 +744,8 @@
       <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:04:45</t>
-        </is>
+      <c r="A20" s="2" t="n">
+        <v>45978.37829861111</v>
       </c>
       <c r="B20" t="n">
         <v>41.1</v>
@@ -794,10 +760,8 @@
       <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:04:55</t>
-        </is>
+      <c r="A21" s="2" t="n">
+        <v>45978.37841435185</v>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
@@ -810,10 +774,8 @@
       <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:05:05</t>
-        </is>
+      <c r="A22" s="2" t="n">
+        <v>45978.3785300926</v>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
@@ -826,10 +788,8 @@
       <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:05:25</t>
-        </is>
+      <c r="A23" s="2" t="n">
+        <v>45978.37876157407</v>
       </c>
       <c r="B23" t="n">
         <v>37</v>
@@ -842,10 +802,8 @@
       <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:05:45</t>
-        </is>
+      <c r="A24" s="2" t="n">
+        <v>45978.37899305556</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
@@ -858,10 +816,8 @@
       <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:06:25</t>
-        </is>
+      <c r="A25" s="2" t="n">
+        <v>45978.37945601852</v>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
@@ -878,10 +834,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:06:35</t>
-        </is>
+      <c r="A26" s="2" t="n">
+        <v>45978.37957175926</v>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
@@ -894,10 +848,8 @@
       <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:06:40</t>
-        </is>
+      <c r="A27" s="2" t="n">
+        <v>45978.37962962963</v>
       </c>
       <c r="B27" t="n">
         <v>43.9</v>
@@ -914,10 +866,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:07:20</t>
-        </is>
+      <c r="A28" s="2" t="n">
+        <v>45978.38009259259</v>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
@@ -928,10 +878,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:07:30</t>
-        </is>
+      <c r="A29" s="2" t="n">
+        <v>45978.38020833334</v>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
@@ -944,10 +892,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:07:40</t>
-        </is>
+      <c r="A30" s="2" t="n">
+        <v>45978.38032407407</v>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="n">
@@ -960,10 +906,8 @@
       <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:08:00</t>
-        </is>
+      <c r="A31" s="2" t="n">
+        <v>45978.38055555556</v>
       </c>
       <c r="B31" t="n">
         <v>40.8</v>
@@ -978,10 +922,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:08:20</t>
-        </is>
+      <c r="A32" s="2" t="n">
+        <v>45978.38078703704</v>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
@@ -994,10 +936,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:08:40</t>
-        </is>
+      <c r="A33" s="2" t="n">
+        <v>45978.38101851852</v>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="n">
@@ -1012,10 +952,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:09:20</t>
-        </is>
+      <c r="A34" s="2" t="n">
+        <v>45978.38148148148</v>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="n">
@@ -1028,10 +966,8 @@
       <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:09:30</t>
-        </is>
+      <c r="A35" s="2" t="n">
+        <v>45978.38159722222</v>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="n">
@@ -1046,10 +982,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:09:40</t>
-        </is>
+      <c r="A36" s="2" t="n">
+        <v>45978.38171296296</v>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
@@ -1060,10 +994,8 @@
       <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:09:55</t>
-        </is>
+      <c r="A37" s="2" t="n">
+        <v>45978.38188657408</v>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
@@ -1072,10 +1004,8 @@
       <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:10:35</t>
-        </is>
+      <c r="A38" s="2" t="n">
+        <v>45978.38234953704</v>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
@@ -1086,10 +1016,8 @@
       <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:11:05</t>
-        </is>
+      <c r="A39" s="2" t="n">
+        <v>45978.38269675926</v>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
@@ -1100,10 +1028,8 @@
       <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:11:15</t>
-        </is>
+      <c r="A40" s="2" t="n">
+        <v>45978.3828125</v>
       </c>
       <c r="B40" t="n">
         <v>25.1</v>
@@ -1118,10 +1044,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:11:20</t>
-        </is>
+      <c r="A41" s="2" t="n">
+        <v>45978.38287037037</v>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
@@ -1130,10 +1054,8 @@
       <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:11:50</t>
-        </is>
+      <c r="A42" s="2" t="n">
+        <v>45978.38321759259</v>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="n">
@@ -1146,10 +1068,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:12:00</t>
-        </is>
+      <c r="A43" s="2" t="n">
+        <v>45978.38333333333</v>
       </c>
       <c r="B43" t="n">
         <v>36.9</v>
@@ -1164,10 +1084,8 @@
       <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:12:40</t>
-        </is>
+      <c r="A44" s="2" t="n">
+        <v>45978.38379629629</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="n">
@@ -1184,10 +1102,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:12:50</t>
-        </is>
+      <c r="A45" s="2" t="n">
+        <v>45978.38391203704</v>
       </c>
       <c r="B45" t="n">
         <v>37.5</v>
@@ -1204,10 +1120,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:12:55</t>
-        </is>
+      <c r="A46" s="2" t="n">
+        <v>45978.38396990741</v>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="n">
@@ -1220,10 +1134,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:13:05</t>
-        </is>
+      <c r="A47" s="2" t="n">
+        <v>45978.38408564815</v>
       </c>
       <c r="B47" t="n">
         <v>31</v>
@@ -1238,10 +1150,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:13:20</t>
-        </is>
+      <c r="A48" s="2" t="n">
+        <v>45978.38425925926</v>
       </c>
       <c r="B48" t="n">
         <v>40.9</v>
@@ -1254,10 +1164,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:13:50</t>
-        </is>
+      <c r="A49" s="2" t="n">
+        <v>45978.38460648148</v>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
@@ -1270,10 +1178,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:14:00</t>
-        </is>
+      <c r="A50" s="2" t="n">
+        <v>45978.38472222222</v>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
@@ -1284,10 +1190,8 @@
       <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>2025-11-17 09:14:05</t>
-        </is>
+      <c r="A51" s="2" t="n">
+        <v>45978.38478009259</v>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="n">

</xml_diff>